<commit_message>
feat(fpu): add support for 32 bit multiplication #2
</commit_message>
<xml_diff>
--- a/programs/pipelining/fpu32bitsmul.xlsx
+++ b/programs/pipelining/fpu32bitsmul.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\pipelining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA07661E-016C-4D2F-8112-E707A231AA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3ADB1EA-665C-4EF1-9F8A-19ACB5E90932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="1" r:id="rId1"/>
@@ -628,18 +628,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E17FB6-AC76-4C3E-BEFA-6AB3607784FD}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="22.7890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="C1">
         <v>15</v>
       </c>
@@ -689,7 +691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -724,7 +726,7 @@
       <c r="Q2" s="10"/>
       <c r="R2" s="10"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -761,7 +763,7 @@
       </c>
       <c r="R3" s="10"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -804,7 +806,7 @@
       </c>
       <c r="R4" s="10"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -831,7 +833,7 @@
       <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
         <v>33</v>
       </c>
@@ -868,7 +870,7 @@
       </c>
       <c r="R6" s="10"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="10" t="s">
         <v>40</v>
       </c>
@@ -891,7 +893,7 @@
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="3"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -912,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -972,7 +974,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1032,7 +1034,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1092,7 +1094,7 @@
         <v>B47</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1121,7 +1123,7 @@
         <v>1</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -1149,10 +1151,10 @@
       </c>
       <c r="S12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>F43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+        <v>E43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1212,7 +1214,7 @@
         <v>13C0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1220,28 +1222,28 @@
         <v>56</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -1269,10 +1271,10 @@
       </c>
       <c r="S14" s="2" t="str">
         <f t="shared" ref="S14" si="1">DEC2HEX(C14*2^15 + D14*2^14 + E14*2^13 + F14*2^12 + G14*2^11 + H14*2^10 + I14*2^9 + J14*2^8 + K14*2^7 + L14*2^6 + M14*2^5 + N14*2^4 + O14 * 2 ^ 3 + P14  * 2^2 + Q14 * 2 + R14)</f>
-        <v>CC82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1332,7 +1334,7 @@
         <v>1E21</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1392,7 +1394,7 @@
         <v>1B00</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1439,7 +1441,7 @@
         <v>0</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q17">
         <v>0</v>
@@ -1449,10 +1451,10 @@
       </c>
       <c r="S17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>C000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+        <v>C004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1512,7 +1514,7 @@
         <v>D44</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1572,7 +1574,7 @@
         <v>D44</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1632,10 +1634,10 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="S21" s="2"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="10" t="s">
         <v>41</v>
       </c>
@@ -1658,7 +1660,7 @@
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
     </row>
-    <row r="23" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1718,7 +1720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1747,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K24" s="9">
         <v>1</v>
@@ -1756,7 +1758,7 @@
         <v>1</v>
       </c>
       <c r="M24" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" s="9">
         <v>0</v>
@@ -1774,11 +1776,11 @@
         <v>0</v>
       </c>
       <c r="S24" s="4" t="str">
-        <f>DEC2HEX(C24*2^15 + D24*2^14 + E24*2^13 + F24*2^12 + G24*2^11 + H24*2^10 + I24*2^9 + J24*2^8 + K24*2^7 + L24*2^6 + M24*2^5 + N24*2^4 + O24 * 2 ^ 3 + P24  * 2^2 + Q24 * 2 + R24)</f>
-        <v>41C0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+        <f t="shared" ref="S24:S28" si="2">DEC2HEX(C24*2^15 + D24*2^14 + E24*2^13 + F24*2^12 + G24*2^11 + H24*2^10 + I24*2^9 + J24*2^8 + K24*2^7 + L24*2^6 + M24*2^5 + N24*2^4 + O24 * 2 ^ 3 + P24  * 2^2 + Q24 * 2 + R24)</f>
+        <v>40E0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1834,11 +1836,11 @@
         <v>0</v>
       </c>
       <c r="S25" s="4" t="str">
-        <f>DEC2HEX(C25*2^15 + D25*2^14 + E25*2^13 + F25*2^12 + G25*2^11 + H25*2^10 + I25*2^9 + J25*2^8 + K25*2^7 + L25*2^6 + M25*2^5 + N25*2^4 + O25 * 2 ^ 3 + P25  * 2^2 + Q25 * 2 + R25)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1867,13 +1869,13 @@
         <v>0</v>
       </c>
       <c r="J26" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26" s="9">
         <v>1</v>
       </c>
       <c r="L26" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M26" s="9">
         <v>0</v>
@@ -1894,11 +1896,11 @@
         <v>0</v>
       </c>
       <c r="S26" s="4" t="str">
-        <f>DEC2HEX(C26*2^15 + D26*2^14 + E26*2^13 + F26*2^12 + G26*2^11 + H26*2^10 + I26*2^9 + J26*2^8 + K26*2^7 + L26*2^6 + M26*2^5 + N26*2^4 + O26 * 2 ^ 3 + P26  * 2^2 + Q26 * 2 + R26)</f>
-        <v>4180</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>40C0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1953,12 +1955,12 @@
       <c r="R27" s="9">
         <v>0</v>
       </c>
-      <c r="S27" s="2" t="str">
-        <f t="shared" ref="S27:S28" si="2">DEC2HEX(C27*2^15 + D27*2^14 + E27*2^13 + F27*2^12 + G27*2^11 + H27*2^10 + I27*2^9 + J27*2^8 + K27*2^7 + L27*2^6 + M27*2^5 + N27*2^4 + O27 * 2 ^ 3 + P27  * 2^2 + Q27 * 2 + R27)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="S27" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2013,7 +2015,7 @@
       <c r="R28" s="9">
         <v>0</v>
       </c>
-      <c r="S28" s="2" t="str">
+      <c r="S28" s="4" t="str">
         <f t="shared" si="2"/>
         <v>4228</v>
       </c>
@@ -2050,22 +2052,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71D0FB5-FE2B-4468-A391-3F433659BE14}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AE19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="20.21875" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" style="2" customWidth="1"/>
-    <col min="4" max="26" width="7.44140625" style="2" customWidth="1"/>
-    <col min="27" max="29" width="5.44140625" style="2" customWidth="1"/>
-    <col min="30" max="30" width="5.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.20703125" customWidth="1"/>
+    <col min="3" max="3" width="12.5234375" style="2" customWidth="1"/>
+    <col min="4" max="26" width="7.41796875" style="2" customWidth="1"/>
+    <col min="27" max="29" width="5.41796875" style="2" customWidth="1"/>
+    <col min="30" max="30" width="5.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="10" t="s">
         <v>46</v>
       </c>
@@ -2102,7 +2105,7 @@
       <c r="Z1" s="5"/>
       <c r="AC1"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -2169,7 +2172,7 @@
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2192,7 +2195,7 @@
       </c>
       <c r="AD3" s="2"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2217,7 +2220,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2242,7 +2245,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -2252,7 +2255,7 @@
       </c>
       <c r="C6" s="2" t="str">
         <f>Code!S12</f>
-        <v>F43</v>
+        <v>E43</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>42</v>
@@ -2267,7 +2270,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -2289,7 +2292,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -2299,7 +2302,7 @@
       </c>
       <c r="C8" s="2" t="str">
         <f>Code!S14</f>
-        <v>CC82</v>
+        <v>1382</v>
       </c>
       <c r="L8" s="4" t="s">
         <v>42</v>
@@ -2312,7 +2315,7 @@
       </c>
       <c r="AC8"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -2338,7 +2341,7 @@
       </c>
       <c r="AC9"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -2361,7 +2364,7 @@
       </c>
       <c r="AC10"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -2371,7 +2374,7 @@
       </c>
       <c r="C11" s="2" t="str">
         <f>Code!S17</f>
-        <v>C000</v>
+        <v>C004</v>
       </c>
       <c r="P11" s="4" t="s">
         <v>42</v>
@@ -2385,7 +2388,7 @@
       <c r="AB11"/>
       <c r="AC11"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -2412,7 +2415,7 @@
       <c r="AB12"/>
       <c r="AC12"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -2439,7 +2442,7 @@
       <c r="AB13"/>
       <c r="AC13"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -2462,16 +2465,16 @@
       </c>
       <c r="AC14"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="AC15"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="AC16"/>
     </row>
-    <row r="17" spans="4:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:29" x14ac:dyDescent="0.55000000000000004">
       <c r="AC17"/>
     </row>
-    <row r="19" spans="4:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:29" x14ac:dyDescent="0.55000000000000004">
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>

</xml_diff>